<commit_message>
updated process mgmt demo
</commit_message>
<xml_diff>
--- a/res/workbook.xlsx
+++ b/res/workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPeterson\OneDrive - Excel Engineering, Inc\documents\repos\pwsh_sandbox\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D00C0861-DEAD-41BF-917C-AA43574A1BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2707614-A6D9-4DB5-BF3A-89EF1B10811E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" xr2:uid="{8AC75AF8-944C-4C87-A622-30FEC0AB98F6}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" xr2:uid="{72C051BC-705B-44CE-AB52-D6B7DF1787C4}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="1">
   <si>
     <t>next empty cell</t>
   </si>
@@ -389,8 +389,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CA7A5E7-824A-4324-930F-E67918FCD209}">
-  <dimension ref="A1:A12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E039E24E-8863-430B-97E5-18CBE7A8A376}">
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,6 +456,16 @@
         <v>0</v>
       </c>
     </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>